<commit_message>
Feature analysis results added. Currently just Bag of Words.
</commit_message>
<xml_diff>
--- a/First10K/FeatureAnalysisResults.xlsx
+++ b/First10K/FeatureAnalysisResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mukund\Documents\College\Grad School Docs\Sem1\Social Computing\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96965CE-73B9-4E5D-BDC4-A4B48539A81C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED40469-BAFB-4357-AD1E-C948D9BC6EF5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9000" xr2:uid="{3D697B4A-49C1-4685-881E-88059CFBC4A7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Model</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Support Vector Classifier</t>
-  </si>
-  <si>
     <t>Accuracy on First 5k</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Recall on First 5k</t>
   </si>
   <si>
-    <t>Bag of Words Feature</t>
-  </si>
-  <si>
     <t>Accuracy on Last 5k</t>
   </si>
   <si>
@@ -66,6 +60,90 @@
   </si>
   <si>
     <t>Recall on Last 5k</t>
+  </si>
+  <si>
+    <t>Bag of Words Feature (Per-Fold Values)</t>
+  </si>
+  <si>
+    <t>[0.48702595, 0.4491018, 0.45, 0.484, 0.49, 0.458, 0.506, 0.482, 0.46292585, 0.43286573]</t>
+  </si>
+  <si>
+    <t>[0.14285714, 0.20141343, 0.164, 0.18410042,0.20634921, 0.172, 0.23282443, 0.1984127, 0.18110236, 0.16853933]</t>
+  </si>
+  <si>
+    <t>[0.51896208, 0.54091816, 0.526, 0.546, 0.538, 0.516, 0.542, 0.51703407, 0.501002]</t>
+  </si>
+  <si>
+    <t>[0.17272727, 0.14054054, 0.17368421, 0.1728972, 0.17821782, 0.17156863, 0.1563981, 0.16326531, 0.11640212, 0.14746544]</t>
+  </si>
+  <si>
+    <t>[0.28037383, 0.53271028, 0.38317757, 0.41121495, 0.48598131, 0.40186916, 0.57009346  0.46728972  0.43396226  0.4245283]</t>
+  </si>
+  <si>
+    <t>[0.39175258, 0.26804124, 0.34020619, 0.3814433, 0.37113402, 0.36082474, 0.34020619  0.32989691  0.22916667  0.33333333]</t>
+  </si>
+  <si>
+    <t>[0.79840319, 0.77644711, 0.788, 0.786, 0.774, 0.78, 0.788, 0.782, 0.78757515, 0.77955912]</t>
+  </si>
+  <si>
+    <t>[0.79640719, 0.80439122, 0.8, 0.806, 0.808, 0.798, 0.812, 0.796, 0.81162325, 0.80360721]</t>
+  </si>
+  <si>
+    <t>[0.41666667, 0.45833333, 0.09090909, 0.5, 0.6, 0.58333333, 0.4, 0.33333333, 0.46153846, 0.41666667]</t>
+  </si>
+  <si>
+    <t>[0.17757009, 0.02803738, 0.06542056, 0.05607477, 0.04672897, 0.04672897, 0.05607477, 0.03738318, 0.08490566, 0.10377358]</t>
+  </si>
+  <si>
+    <t>[0.04123711, 0.08247423, 0.02061856, 0.04123711, 0.04123711, 0.02061856, 0.03092784, 0.08247423, 0.0625, 0.0625]</t>
+  </si>
+  <si>
+    <t>[0.77045908, 0.75449102, 0.756, 0.736, 0.738, 0.742, 0.752, 0.754, 0.77955912, 0.75551102]</t>
+  </si>
+  <si>
+    <t>[0.74850299, 0.76247505, 0.756, 0.806, 0.76, 0.758, 0.788, 0.764, 0.76953908, 0.7995992]</t>
+  </si>
+  <si>
+    <t>[0.45454545, 0.38571429, 0.4137931, 0.29508197, 0.25, 0.31666667, 0.33962264, 0.32608696, 0.46551724, 0.35714286]</t>
+  </si>
+  <si>
+    <t>[0.28985507, 0.35526316, 0.22222222, 0.5, 0.26530612, 0.3125, 0.36363636, 0.26666667, 0.35820896, 0.45454545]</t>
+  </si>
+  <si>
+    <t>[0.20618557, 0.27835052, 0.10309278, 0.22680412, 0.13402062, 0.20618557, 0.12371134, 0.12371134, 0.25, 0.20833333]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>[0.28282828, 0.30630631, 0.24050633, 0.36486486, 0.26582278, 0.27586207, 0.35064935, 0.25925926, 0.32323232, 0.33333333]</t>
+  </si>
+  <si>
+    <t>[0.37383178, 0.25233645, 0.3364486, 0.1682243, 0.11214953, 0.17757009, 0.1682243, 0.14018692, 0.25471698, 0.18867925]</t>
+  </si>
+  <si>
+    <t>[0.39252336, 0.31775701, 0.40186916, 0.24299065, 0.17757009, 0.20560748, 0.25233645, 0.23364486, 0.31132075, 0.24528302]</t>
+  </si>
+  <si>
+    <t>[0.28865979, 0.35051546, 0.19587629, 0.27835052, 0.21649485, 0.24742268, 0.27835052, 0.21649485, 0.33333333, 0.27083333]</t>
+  </si>
+  <si>
+    <t>[0.73253493, 0.71457086, 0.714, 0.7, 0.71, 0.7, 0.716, 0.74, 0.73547094, 0.71142285]</t>
+  </si>
+  <si>
+    <t>[0.72055888, 0.72055888, 0.724, 0.766, 0.732, 0.728, 0.76, 0.728, 0.73747495, 0.75551102]</t>
+  </si>
+  <si>
+    <t>[0.5625, 0.46153846, 0.5, 0.6, 0.375, 0.26666667, 0.5, 0.38461538, 0.66666667, 0.56]</t>
+  </si>
+  <si>
+    <t>[0.37837838, 0.32692308, 0.35245902, 0.27368421, 0.25, 0.25287356, 0.30337079, 0.34246575, 0.35869565, 0.28888889]</t>
+  </si>
+  <si>
+    <t>Support Vector Classifier (Linear Kernel)</t>
+  </si>
+  <si>
+    <t>Bag of Words Feature (Average Results)</t>
   </si>
 </sst>
 </file>
@@ -138,16 +216,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,152 +557,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E449D2EB-30BC-425C-A5F7-643CEFD9A346}">
-  <dimension ref="B2:H7"/>
+  <dimension ref="B2:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="102.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="108.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+    <row r="2" spans="2:17">
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:17">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
+      <c r="P3" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:17">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
-        <v>0.97660000000000002</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.311764705882</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.210526315789</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="C4" s="3">
+        <v>0.47019193300000001</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.52732403444443998</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.18515990199999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.159316664</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.43912008400000002</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.33460051699999999</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:17">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.998</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.99760000000000004</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.81132075471700005</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.66666666666700003</v>
-      </c>
+      <c r="C5" s="3">
+        <v>0.78399845700000004</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.80360288700000004</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.48769871799999998</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.42607808800000002</v>
+      </c>
+      <c r="G5" s="3">
+        <v>7.0269792999999997E-2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4.8582475E-2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:17">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.999</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.999</v>
+      <c r="C6" s="4">
+        <v>0.75380202399999996</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.77121163199999998</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>0.36041711799999998</v>
       </c>
       <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.90566037735799998</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.86111111111100003</v>
-      </c>
+        <v>0.33882040099999999</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.21723682</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.18603951899999999</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:17">
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>0.717399958</v>
       </c>
       <c r="D7" s="3">
-        <v>1</v>
+        <v>0.73721037300000003</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>0.312773933</v>
       </c>
       <c r="F7" s="3">
-        <v>1</v>
+        <v>0.30026648900000003</v>
       </c>
       <c r="G7" s="3">
-        <v>1</v>
+        <v>0.27809028299999999</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
-      </c>
+        <v>0.26763316199999998</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="K9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="K10" s="6"/>
+      <c r="N10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:H2"/>
+    <mergeCell ref="J2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added data for TF-IDF Scores.
</commit_message>
<xml_diff>
--- a/First10K/FeatureAnalysisResults.xlsx
+++ b/First10K/FeatureAnalysisResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mukund\Documents\College\Grad School Docs\Sem1\Social Computing\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED40469-BAFB-4357-AD1E-C948D9BC6EF5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E16708F-ED09-4A7C-B37A-E1A1ADD65CD7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9000" xr2:uid="{3D697B4A-49C1-4685-881E-88059CFBC4A7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Model</t>
   </si>
@@ -144,6 +144,84 @@
   </si>
   <si>
     <t>Bag of Words Feature (Average Results)</t>
+  </si>
+  <si>
+    <t>[0.51297405, 0.4750499, 0.488, 0.488, 0.504, 0.464, 0.502, 0.504, 0.4749499, 0.46092184]</t>
+  </si>
+  <si>
+    <t>[0.52095808, 0.56287425, 0.572, 0.54, 0.56, 0.542, 0.54, 0.548, 0.53907816, 0.52104208]</t>
+  </si>
+  <si>
+    <t>[0.14507772, 0.20895522, 0.17180617, 0.18025751, 0.2, 0.16872428, 0.21825397, 0.20502092, 0.17226891, 0.16734694]</t>
+  </si>
+  <si>
+    <t>[0.15458937, 0.14534884, 0.17318436, 0.17241379, 0.18461538, 0.16666667, 0.16915423, 0.16230366, 0.11931818, 0.15458937]</t>
+  </si>
+  <si>
+    <t>[0.26168224, 0.52336449, 0.36448598, 0.39252336, 0.43925234, 0.38317757, 0.51401869, 0.45794393, 0.38679245, 0.38679245]</t>
+  </si>
+  <si>
+    <t>[0.32989691, 0.25773196, 0.31958763, 0.36082474, 0.37113402, 0.34020619, 0.35051546, 0.31958763, 0.21875, 0.33333333]</t>
+  </si>
+  <si>
+    <t>[0.78642715, 0.78243513, 0.786, 0.79, 0.782, 0.786, 0.788, 0.782, 0.77955912, 0.80160321]</t>
+  </si>
+  <si>
+    <t>[0.72727273, 0.22222222, 0.375, 0.66666667, 0.5, 0.5, 0.28571429, 0.14285714, 0.55555556, 0.6]</t>
+  </si>
+  <si>
+    <t>[0.11214953, 0.01869159, 0.02803738, 0.04672897, 0.01869159, 0.03738318, 0.01869159, 0.01869159, 0.01886792, 0.06603774]</t>
+  </si>
+  <si>
+    <t>[0.80638723, 0.80439122, 0.8, 0.804, 0.802, 0.798, 0.806, 0.804, 0.80761523, 0.80961924]</t>
+  </si>
+  <si>
+    <t>[0.5, 0.66666667, 0.0, 0.0, 1.0, 0.0, 0.33333333, 0.25, 0.33333333, 0.0]</t>
+  </si>
+  <si>
+    <t>[0.0, 0.02061856, 0.01030928, 0.01030928, 0.0, 0.01030928, 0.0, 0.03092784, 0.04166667, 0.01041667]</t>
+  </si>
+  <si>
+    <t>[0.80838323, 0.78443114, 0.788, 0.782, 0.784, 0.792, 0.788, 0.782, 0.78957916, 0.79158317]</t>
+  </si>
+  <si>
+    <t>[0.78947368, 0.42857143, 0.54545455, 0.42857143, 0.33333333, 0.66666667, 0.66666667, 0.25, 0.55555556, 0.55]</t>
+  </si>
+  <si>
+    <t>[0.80239521, 0.80838323, 0.804, 0.808, 0.81, 0.806, 0.808, 0.816, 0.81162325, 0.81362725]</t>
+  </si>
+  <si>
+    <t>[0.25, 0.6, 0.33333333, 1.0, 0.75, 0.5, 1.0, 1.0, 1.0, 0.8]</t>
+  </si>
+  <si>
+    <t>[0.14018692, 0.02803738, 0.05607477, 0.05607477, 0.00934579, 0.05607477, 0.01869159, 0.00934579, 0.04716981, 0.10377358]</t>
+  </si>
+  <si>
+    <t>[0.01030928, 0.03092784, 0.01030928, 0.01030928, 0.03092784, 0.01030928, 0.01030928, 0.05154639, 0.02083333, 0.04166667]</t>
+  </si>
+  <si>
+    <t>[0.79041916, 0.77844311, 0.79, 0.772, 0.786, 0.79, 0.782, 0.786, 0.78356713, 0.7995992]</t>
+  </si>
+  <si>
+    <t>[0.58333333, 0.3, 0.66666667, 0.23076923, 0.5, 0.66666667, 0.25, 0.5, 0.33333333, 0.6875]</t>
+  </si>
+  <si>
+    <t>[0.06542056, 0.02803738, 0.03738318, 0.02803738, 0.01869159, 0.03738318, 0.00934579, 0.01869159, 0.01886792, 0.10377358]</t>
+  </si>
+  <si>
+    <t>[0.80439122, 0.80638723, 0.806, 0.808, 0.812, 0.806, 0.806, 0.808, 0.80761523, 0.80961924]</t>
+  </si>
+  <si>
+    <t>[0.33333333, 0.5, 0.0, 1.0, 1.0, 0.0, 0.5, 1.0, 0.0, 1.0]</t>
+  </si>
+  <si>
+    <t>[0.01030928, 0.02061856, 0.0, 0.01030928, 0.03092784, 0.0, 0.01030928, 0.01030928, 0.0, 0.01041667]</t>
+  </si>
+  <si>
+    <t>TF-IDF Feature (Average Results)</t>
+  </si>
+  <si>
+    <t>TF-IDF Feature (Per-Fold Values)</t>
   </si>
 </sst>
 </file>
@@ -216,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -231,9 +309,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -557,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E449D2EB-30BC-425C-A5F7-643CEFD9A346}">
-  <dimension ref="B2:Q10"/>
+  <dimension ref="B2:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -574,7 +649,7 @@
     <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="77.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="83.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="102.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="108.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -674,19 +749,19 @@
       <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="9"/>
+      <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="2" t="s">
@@ -713,25 +788,25 @@
       <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="8"/>
     </row>
     <row r="6" spans="2:17">
       <c r="B6" s="2" t="s">
@@ -758,25 +833,25 @@
       <c r="J6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="2:17">
       <c r="B7" s="2" t="s">
@@ -803,25 +878,25 @@
       <c r="J7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="2:17">
       <c r="K8" s="6"/>
@@ -834,17 +909,259 @@
       <c r="P8" s="6"/>
     </row>
     <row r="9" spans="2:17">
-      <c r="K9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
     </row>
     <row r="10" spans="2:17">
-      <c r="K10" s="6"/>
-      <c r="N10" s="8"/>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.48738956900000002</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.544595257</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.18377116399999999</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.16021838499999999</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.41100334999999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.320156787</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.786402461</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.80420129200000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.45752886100000001</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.30833333299999999</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3.8397107999999999E-2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.3455758E-2</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.78899766999999998</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.80880289400000005</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.52142933199999997</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.72333333300000002</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5.2477517000000001E-2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2.2744846999999999E-2</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.78580285999999999</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.80740129199999999</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.34474358999999999</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.53333333299999997</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1.9643800999999999E-2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.0320019E-2</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="J2:P2"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>